<commit_message>
Adding a few more files for questions to be uploaded
</commit_message>
<xml_diff>
--- a/src/main/resources/questions/Numbers.xlsx
+++ b/src/main/resources/questions/Numbers.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="742" uniqueCount="14">
   <si>
     <t xml:space="preserve">CourseName</t>
   </si>
@@ -171,19 +171,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F105"/>
+  <dimension ref="A1:F185"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I19" activeCellId="0" sqref="I19"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A76" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F28" activeCellId="0" sqref="F28:F107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.1740890688259"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.0323886639676"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.2834008097166"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.1376518218623"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="7.81781376518219"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.9595141700405"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.4251012145749"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.0688259109312"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.5303643724696"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="7.49797570850202"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.57085020242915"/>
   </cols>
@@ -733,19 +733,19 @@
         <v>6</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C28" s="0" t="n">
-        <v>50900</v>
+        <v>58766</v>
       </c>
       <c r="D28" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F28" s="0" t="n">
-        <v>50900</v>
+        <v>58766</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -753,19 +753,19 @@
         <v>6</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C29" s="0" t="n">
-        <v>50901</v>
+        <v>58767</v>
       </c>
       <c r="D29" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F29" s="0" t="n">
-        <v>50901</v>
+        <v>58767</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -773,19 +773,19 @@
         <v>6</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C30" s="0" t="n">
-        <v>50902</v>
+        <v>58768</v>
       </c>
       <c r="D30" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F30" s="0" t="n">
-        <v>50902</v>
+        <v>58768</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -793,19 +793,19 @@
         <v>6</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C31" s="0" t="n">
-        <v>50903</v>
+        <v>58769</v>
       </c>
       <c r="D31" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F31" s="0" t="n">
-        <v>50903</v>
+        <v>58769</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -813,19 +813,19 @@
         <v>6</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C32" s="0" t="n">
-        <v>100000</v>
+        <v>58770</v>
       </c>
       <c r="D32" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F32" s="0" t="n">
-        <v>100000</v>
+        <v>58770</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -833,19 +833,19 @@
         <v>6</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C33" s="0" t="n">
-        <v>100001</v>
+        <v>58771</v>
       </c>
       <c r="D33" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F33" s="0" t="n">
-        <v>100001</v>
+        <v>58771</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -853,19 +853,19 @@
         <v>6</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C34" s="0" t="n">
-        <v>100002</v>
+        <v>58772</v>
       </c>
       <c r="D34" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F34" s="0" t="n">
-        <v>100002</v>
+        <v>58772</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -873,19 +873,19 @@
         <v>6</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C35" s="0" t="n">
-        <v>100003</v>
+        <v>58773</v>
       </c>
       <c r="D35" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F35" s="0" t="n">
-        <v>100003</v>
+        <v>58773</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -893,19 +893,19 @@
         <v>6</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C36" s="0" t="n">
-        <v>100004</v>
+        <v>58774</v>
       </c>
       <c r="D36" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F36" s="0" t="n">
-        <v>100004</v>
+        <v>58774</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -913,19 +913,19 @@
         <v>6</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C37" s="0" t="n">
-        <v>100005</v>
+        <v>58775</v>
       </c>
       <c r="D37" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F37" s="0" t="n">
-        <v>100005</v>
+        <v>58775</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -933,19 +933,19 @@
         <v>6</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C38" s="0" t="n">
-        <v>100006</v>
+        <v>58776</v>
       </c>
       <c r="D38" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F38" s="0" t="n">
-        <v>100006</v>
+        <v>58776</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -953,19 +953,19 @@
         <v>6</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C39" s="0" t="n">
-        <v>100007</v>
+        <v>58777</v>
       </c>
       <c r="D39" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F39" s="0" t="n">
-        <v>100007</v>
+        <v>58777</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -973,19 +973,19 @@
         <v>6</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C40" s="0" t="n">
-        <v>100008</v>
+        <v>58778</v>
       </c>
       <c r="D40" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E40" s="0" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F40" s="0" t="n">
-        <v>100008</v>
+        <v>58778</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -993,19 +993,19 @@
         <v>6</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C41" s="0" t="n">
-        <v>100009</v>
+        <v>58779</v>
       </c>
       <c r="D41" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E41" s="0" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F41" s="0" t="n">
-        <v>100009</v>
+        <v>58779</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1013,19 +1013,19 @@
         <v>6</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C42" s="0" t="n">
-        <v>100010</v>
+        <v>58780</v>
       </c>
       <c r="D42" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E42" s="0" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F42" s="0" t="n">
-        <v>100010</v>
+        <v>58780</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1033,19 +1033,19 @@
         <v>6</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C43" s="0" t="n">
-        <v>100011</v>
+        <v>58781</v>
       </c>
       <c r="D43" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E43" s="0" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F43" s="0" t="n">
-        <v>100011</v>
+        <v>58781</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1053,19 +1053,19 @@
         <v>6</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C44" s="0" t="n">
-        <v>100012</v>
+        <v>58782</v>
       </c>
       <c r="D44" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E44" s="0" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F44" s="0" t="n">
-        <v>100012</v>
+        <v>58782</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1073,19 +1073,19 @@
         <v>6</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C45" s="0" t="n">
-        <v>950</v>
+        <v>58783</v>
       </c>
       <c r="D45" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E45" s="0" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F45" s="0" t="n">
-        <v>950</v>
+        <v>58783</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1093,19 +1093,19 @@
         <v>6</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C46" s="0" t="n">
-        <v>951</v>
+        <v>58784</v>
       </c>
       <c r="D46" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E46" s="0" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F46" s="0" t="n">
-        <v>951</v>
+        <v>58784</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1113,19 +1113,19 @@
         <v>6</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C47" s="0" t="n">
-        <v>952</v>
+        <v>6211</v>
       </c>
       <c r="D47" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E47" s="0" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F47" s="0" t="n">
-        <v>952</v>
+        <v>6211</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1133,19 +1133,19 @@
         <v>6</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C48" s="0" t="n">
-        <v>953</v>
+        <v>6212</v>
       </c>
       <c r="D48" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E48" s="0" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F48" s="0" t="n">
-        <v>953</v>
+        <v>6212</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1153,19 +1153,19 @@
         <v>6</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C49" s="0" t="n">
-        <v>954</v>
+        <v>6213</v>
       </c>
       <c r="D49" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E49" s="0" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F49" s="0" t="n">
-        <v>954</v>
+        <v>6213</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1173,19 +1173,19 @@
         <v>6</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C50" s="0" t="n">
-        <v>955</v>
+        <v>6214</v>
       </c>
       <c r="D50" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E50" s="0" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F50" s="0" t="n">
-        <v>955</v>
+        <v>6214</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1193,19 +1193,19 @@
         <v>6</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C51" s="0" t="n">
-        <v>956</v>
+        <v>6215</v>
       </c>
       <c r="D51" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E51" s="0" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F51" s="0" t="n">
-        <v>956</v>
+        <v>6215</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1213,19 +1213,19 @@
         <v>6</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C52" s="0" t="n">
-        <v>957</v>
+        <v>6216</v>
       </c>
       <c r="D52" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E52" s="0" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F52" s="0" t="n">
-        <v>957</v>
+        <v>6216</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1233,19 +1233,19 @@
         <v>6</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C53" s="0" t="n">
-        <v>958</v>
+        <v>6217</v>
       </c>
       <c r="D53" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E53" s="0" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F53" s="0" t="n">
-        <v>958</v>
+        <v>6217</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1253,19 +1253,19 @@
         <v>6</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C54" s="0" t="n">
-        <v>959</v>
+        <v>6218</v>
       </c>
       <c r="D54" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E54" s="0" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F54" s="0" t="n">
-        <v>959</v>
+        <v>6218</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1273,19 +1273,19 @@
         <v>6</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C55" s="0" t="n">
-        <v>960</v>
+        <v>6219</v>
       </c>
       <c r="D55" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E55" s="0" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F55" s="0" t="n">
-        <v>960</v>
+        <v>6219</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1293,19 +1293,19 @@
         <v>6</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C56" s="0" t="n">
-        <v>725</v>
+        <v>6220</v>
       </c>
       <c r="D56" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E56" s="0" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F56" s="0" t="n">
-        <v>725</v>
+        <v>6220</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1313,19 +1313,19 @@
         <v>6</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C57" s="0" t="n">
-        <v>726</v>
+        <v>6221</v>
       </c>
       <c r="D57" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E57" s="0" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F57" s="0" t="n">
-        <v>726</v>
+        <v>6221</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1333,19 +1333,19 @@
         <v>6</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C58" s="0" t="n">
-        <v>727</v>
+        <v>6222</v>
       </c>
       <c r="D58" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E58" s="0" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F58" s="0" t="n">
-        <v>727</v>
+        <v>6222</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1353,19 +1353,19 @@
         <v>6</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C59" s="0" t="n">
-        <v>728</v>
+        <v>6223</v>
       </c>
       <c r="D59" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E59" s="0" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F59" s="0" t="n">
-        <v>728</v>
+        <v>6223</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1373,19 +1373,19 @@
         <v>6</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C60" s="0" t="n">
-        <v>729</v>
+        <v>6224</v>
       </c>
       <c r="D60" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E60" s="0" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F60" s="0" t="n">
-        <v>729</v>
+        <v>6224</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1393,19 +1393,19 @@
         <v>6</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C61" s="0" t="n">
-        <v>730</v>
+        <v>122234</v>
       </c>
       <c r="D61" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E61" s="0" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F61" s="0" t="n">
-        <v>730</v>
+        <v>122234</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1413,19 +1413,19 @@
         <v>6</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C62" s="0" t="n">
-        <v>731</v>
+        <v>122235</v>
       </c>
       <c r="D62" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E62" s="0" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F62" s="0" t="n">
-        <v>731</v>
+        <v>122235</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1433,19 +1433,19 @@
         <v>6</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C63" s="0" t="n">
-        <v>732</v>
+        <v>122236</v>
       </c>
       <c r="D63" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E63" s="0" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F63" s="0" t="n">
-        <v>732</v>
+        <v>122236</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1453,19 +1453,19 @@
         <v>6</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C64" s="0" t="n">
-        <v>733</v>
+        <v>122237</v>
       </c>
       <c r="D64" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E64" s="0" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F64" s="0" t="n">
-        <v>733</v>
+        <v>122237</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1473,19 +1473,19 @@
         <v>6</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C65" s="0" t="n">
-        <v>734</v>
+        <v>122238</v>
       </c>
       <c r="D65" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E65" s="0" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F65" s="0" t="n">
-        <v>734</v>
+        <v>122238</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1493,19 +1493,19 @@
         <v>6</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C66" s="0" t="n">
-        <v>333</v>
+        <v>122239</v>
       </c>
       <c r="D66" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E66" s="0" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F66" s="0" t="n">
-        <v>333</v>
+        <v>122239</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1513,19 +1513,19 @@
         <v>6</v>
       </c>
       <c r="B67" s="0" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C67" s="0" t="n">
-        <v>334</v>
+        <v>122240</v>
       </c>
       <c r="D67" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E67" s="0" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F67" s="0" t="n">
-        <v>334</v>
+        <v>122240</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1533,19 +1533,19 @@
         <v>6</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C68" s="0" t="n">
-        <v>335</v>
+        <v>122241</v>
       </c>
       <c r="D68" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E68" s="0" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F68" s="0" t="n">
-        <v>335</v>
+        <v>122241</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1553,19 +1553,19 @@
         <v>6</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C69" s="0" t="n">
-        <v>336</v>
+        <v>122242</v>
       </c>
       <c r="D69" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E69" s="0" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F69" s="0" t="n">
-        <v>336</v>
+        <v>122242</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1573,19 +1573,19 @@
         <v>6</v>
       </c>
       <c r="B70" s="0" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C70" s="0" t="n">
-        <v>337</v>
+        <v>122243</v>
       </c>
       <c r="D70" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E70" s="0" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F70" s="0" t="n">
-        <v>337</v>
+        <v>122243</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1593,19 +1593,19 @@
         <v>6</v>
       </c>
       <c r="B71" s="0" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C71" s="0" t="n">
-        <v>338</v>
+        <v>122244</v>
       </c>
       <c r="D71" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E71" s="0" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F71" s="0" t="n">
-        <v>338</v>
+        <v>122244</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1613,19 +1613,19 @@
         <v>6</v>
       </c>
       <c r="B72" s="0" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C72" s="0" t="n">
-        <v>339</v>
+        <v>122245</v>
       </c>
       <c r="D72" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E72" s="0" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F72" s="0" t="n">
-        <v>339</v>
+        <v>122245</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1633,19 +1633,19 @@
         <v>6</v>
       </c>
       <c r="B73" s="0" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C73" s="0" t="n">
-        <v>340</v>
+        <v>122246</v>
       </c>
       <c r="D73" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E73" s="0" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F73" s="0" t="n">
-        <v>340</v>
+        <v>122246</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1653,19 +1653,19 @@
         <v>6</v>
       </c>
       <c r="B74" s="0" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C74" s="0" t="n">
-        <v>341</v>
+        <v>122247</v>
       </c>
       <c r="D74" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E74" s="0" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F74" s="0" t="n">
-        <v>341</v>
+        <v>122247</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1673,19 +1673,19 @@
         <v>6</v>
       </c>
       <c r="B75" s="0" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C75" s="0" t="n">
-        <v>342</v>
+        <v>122248</v>
       </c>
       <c r="D75" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E75" s="0" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F75" s="0" t="n">
-        <v>342</v>
+        <v>122248</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1693,19 +1693,19 @@
         <v>6</v>
       </c>
       <c r="B76" s="0" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C76" s="0" t="n">
-        <v>343</v>
+        <v>122249</v>
       </c>
       <c r="D76" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E76" s="0" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F76" s="0" t="n">
-        <v>343</v>
+        <v>122249</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1713,19 +1713,19 @@
         <v>6</v>
       </c>
       <c r="B77" s="0" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C77" s="0" t="n">
-        <v>344</v>
+        <v>122250</v>
       </c>
       <c r="D77" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E77" s="0" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F77" s="0" t="n">
-        <v>344</v>
+        <v>122250</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1733,19 +1733,19 @@
         <v>6</v>
       </c>
       <c r="B78" s="0" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C78" s="0" t="n">
-        <v>345</v>
+        <v>122251</v>
       </c>
       <c r="D78" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E78" s="0" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F78" s="0" t="n">
-        <v>345</v>
+        <v>122251</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1753,19 +1753,19 @@
         <v>6</v>
       </c>
       <c r="B79" s="0" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C79" s="0" t="n">
-        <v>346</v>
+        <v>122252</v>
       </c>
       <c r="D79" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E79" s="0" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F79" s="0" t="n">
-        <v>346</v>
+        <v>122252</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1773,19 +1773,19 @@
         <v>6</v>
       </c>
       <c r="B80" s="0" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C80" s="0" t="n">
-        <v>347</v>
+        <v>122253</v>
       </c>
       <c r="D80" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E80" s="0" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F80" s="0" t="n">
-        <v>347</v>
+        <v>122253</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1793,19 +1793,19 @@
         <v>6</v>
       </c>
       <c r="B81" s="0" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C81" s="0" t="n">
-        <v>348</v>
+        <v>122254</v>
       </c>
       <c r="D81" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E81" s="0" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F81" s="0" t="n">
-        <v>348</v>
+        <v>122254</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1813,19 +1813,19 @@
         <v>6</v>
       </c>
       <c r="B82" s="0" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C82" s="0" t="n">
-        <v>349</v>
+        <v>122255</v>
       </c>
       <c r="D82" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E82" s="0" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F82" s="0" t="n">
-        <v>349</v>
+        <v>122255</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1833,19 +1833,19 @@
         <v>6</v>
       </c>
       <c r="B83" s="0" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C83" s="0" t="n">
-        <v>350</v>
+        <v>122256</v>
       </c>
       <c r="D83" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E83" s="0" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F83" s="0" t="n">
-        <v>350</v>
+        <v>122256</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1853,19 +1853,19 @@
         <v>6</v>
       </c>
       <c r="B84" s="0" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C84" s="0" t="n">
-        <v>56789</v>
+        <v>122257</v>
       </c>
       <c r="D84" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E84" s="0" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F84" s="0" t="n">
-        <v>56789</v>
+        <v>122257</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1873,19 +1873,19 @@
         <v>6</v>
       </c>
       <c r="B85" s="0" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C85" s="0" t="n">
-        <v>56790</v>
+        <v>122258</v>
       </c>
       <c r="D85" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E85" s="0" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F85" s="0" t="n">
-        <v>56790</v>
+        <v>122258</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1893,19 +1893,19 @@
         <v>6</v>
       </c>
       <c r="B86" s="0" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C86" s="0" t="n">
-        <v>56791</v>
+        <v>122259</v>
       </c>
       <c r="D86" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E86" s="0" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F86" s="0" t="n">
-        <v>56791</v>
+        <v>122259</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1913,19 +1913,19 @@
         <v>6</v>
       </c>
       <c r="B87" s="0" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C87" s="0" t="n">
-        <v>56792</v>
+        <v>122260</v>
       </c>
       <c r="D87" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E87" s="0" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F87" s="0" t="n">
-        <v>56792</v>
+        <v>122260</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1933,19 +1933,19 @@
         <v>6</v>
       </c>
       <c r="B88" s="0" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C88" s="0" t="n">
-        <v>56793</v>
+        <v>122261</v>
       </c>
       <c r="D88" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E88" s="0" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F88" s="0" t="n">
-        <v>56793</v>
+        <v>122261</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1953,19 +1953,19 @@
         <v>6</v>
       </c>
       <c r="B89" s="0" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C89" s="0" t="n">
-        <v>56794</v>
+        <v>122262</v>
       </c>
       <c r="D89" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E89" s="0" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F89" s="0" t="n">
-        <v>56794</v>
+        <v>122262</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1973,19 +1973,19 @@
         <v>6</v>
       </c>
       <c r="B90" s="0" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C90" s="0" t="n">
-        <v>56795</v>
+        <v>122263</v>
       </c>
       <c r="D90" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E90" s="0" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F90" s="0" t="n">
-        <v>56795</v>
+        <v>122263</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1993,19 +1993,19 @@
         <v>6</v>
       </c>
       <c r="B91" s="0" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C91" s="0" t="n">
-        <v>56796</v>
+        <v>122264</v>
       </c>
       <c r="D91" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E91" s="0" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F91" s="0" t="n">
-        <v>56796</v>
+        <v>122264</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2013,19 +2013,19 @@
         <v>6</v>
       </c>
       <c r="B92" s="0" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C92" s="0" t="n">
-        <v>56797</v>
+        <v>122265</v>
       </c>
       <c r="D92" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E92" s="0" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F92" s="0" t="n">
-        <v>56797</v>
+        <v>122265</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2033,19 +2033,19 @@
         <v>6</v>
       </c>
       <c r="B93" s="0" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C93" s="0" t="n">
-        <v>56798</v>
+        <v>122266</v>
       </c>
       <c r="D93" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E93" s="0" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F93" s="0" t="n">
-        <v>56798</v>
+        <v>122266</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2053,19 +2053,19 @@
         <v>6</v>
       </c>
       <c r="B94" s="0" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C94" s="0" t="n">
-        <v>56799</v>
+        <v>122267</v>
       </c>
       <c r="D94" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E94" s="0" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F94" s="0" t="n">
-        <v>56799</v>
+        <v>122267</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2073,19 +2073,19 @@
         <v>6</v>
       </c>
       <c r="B95" s="0" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C95" s="0" t="n">
-        <v>56800</v>
+        <v>90123</v>
       </c>
       <c r="D95" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E95" s="0" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F95" s="0" t="n">
-        <v>56800</v>
+        <v>90123</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2093,19 +2093,19 @@
         <v>6</v>
       </c>
       <c r="B96" s="0" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C96" s="0" t="n">
-        <v>56801</v>
+        <v>90124</v>
       </c>
       <c r="D96" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E96" s="0" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F96" s="0" t="n">
-        <v>56801</v>
+        <v>90124</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2113,19 +2113,19 @@
         <v>6</v>
       </c>
       <c r="B97" s="0" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C97" s="0" t="n">
-        <v>56802</v>
+        <v>90125</v>
       </c>
       <c r="D97" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E97" s="0" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F97" s="0" t="n">
-        <v>56802</v>
+        <v>90125</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2133,19 +2133,19 @@
         <v>6</v>
       </c>
       <c r="B98" s="0" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C98" s="0" t="n">
-        <v>56803</v>
+        <v>90126</v>
       </c>
       <c r="D98" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E98" s="0" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F98" s="0" t="n">
-        <v>56803</v>
+        <v>90126</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2153,19 +2153,19 @@
         <v>6</v>
       </c>
       <c r="B99" s="0" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C99" s="0" t="n">
-        <v>56804</v>
+        <v>90127</v>
       </c>
       <c r="D99" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E99" s="0" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F99" s="0" t="n">
-        <v>56804</v>
+        <v>90127</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2173,19 +2173,19 @@
         <v>6</v>
       </c>
       <c r="B100" s="0" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C100" s="0" t="n">
-        <v>56805</v>
+        <v>90128</v>
       </c>
       <c r="D100" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E100" s="0" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F100" s="0" t="n">
-        <v>56805</v>
+        <v>90128</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2193,19 +2193,19 @@
         <v>6</v>
       </c>
       <c r="B101" s="0" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C101" s="0" t="n">
-        <v>56806</v>
+        <v>90129</v>
       </c>
       <c r="D101" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E101" s="0" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F101" s="0" t="n">
-        <v>56806</v>
+        <v>90129</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2213,19 +2213,19 @@
         <v>6</v>
       </c>
       <c r="B102" s="0" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C102" s="0" t="n">
-        <v>56807</v>
+        <v>90130</v>
       </c>
       <c r="D102" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E102" s="0" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F102" s="0" t="n">
-        <v>56807</v>
+        <v>90130</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2233,19 +2233,19 @@
         <v>6</v>
       </c>
       <c r="B103" s="0" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C103" s="0" t="n">
-        <v>56808</v>
+        <v>90131</v>
       </c>
       <c r="D103" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E103" s="0" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F103" s="0" t="n">
-        <v>56808</v>
+        <v>90131</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2253,19 +2253,19 @@
         <v>6</v>
       </c>
       <c r="B104" s="0" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C104" s="0" t="n">
-        <v>56809</v>
+        <v>90132</v>
       </c>
       <c r="D104" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E104" s="0" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F104" s="0" t="n">
-        <v>56809</v>
+        <v>90132</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2273,18 +2273,1618 @@
         <v>6</v>
       </c>
       <c r="B105" s="0" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C105" s="0" t="n">
+        <v>90133</v>
+      </c>
+      <c r="D105" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E105" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="F105" s="0" t="n">
+        <v>90133</v>
+      </c>
+    </row>
+    <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A106" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B106" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C106" s="0" t="n">
+        <v>90134</v>
+      </c>
+      <c r="D106" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E106" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="F106" s="0" t="n">
+        <v>90134</v>
+      </c>
+    </row>
+    <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A107" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B107" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C107" s="0" t="n">
+        <v>90135</v>
+      </c>
+      <c r="D107" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E107" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="F107" s="0" t="n">
+        <v>90135</v>
+      </c>
+    </row>
+    <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A108" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B108" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C108" s="0" t="n">
+        <v>50900</v>
+      </c>
+      <c r="D108" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E108" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="F108" s="0" t="n">
+        <v>50900</v>
+      </c>
+    </row>
+    <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A109" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B109" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C109" s="0" t="n">
+        <v>50901</v>
+      </c>
+      <c r="D109" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E109" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="F109" s="0" t="n">
+        <v>50901</v>
+      </c>
+    </row>
+    <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A110" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B110" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C110" s="0" t="n">
+        <v>50902</v>
+      </c>
+      <c r="D110" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E110" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="F110" s="0" t="n">
+        <v>50902</v>
+      </c>
+    </row>
+    <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A111" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B111" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C111" s="0" t="n">
+        <v>50903</v>
+      </c>
+      <c r="D111" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E111" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="F111" s="0" t="n">
+        <v>50903</v>
+      </c>
+    </row>
+    <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A112" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B112" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C112" s="0" t="n">
+        <v>100000</v>
+      </c>
+      <c r="D112" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E112" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="F112" s="0" t="n">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A113" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B113" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C113" s="0" t="n">
+        <v>100001</v>
+      </c>
+      <c r="D113" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E113" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="F113" s="0" t="n">
+        <v>100001</v>
+      </c>
+    </row>
+    <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A114" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B114" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C114" s="0" t="n">
+        <v>100002</v>
+      </c>
+      <c r="D114" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E114" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="F114" s="0" t="n">
+        <v>100002</v>
+      </c>
+    </row>
+    <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A115" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B115" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C115" s="0" t="n">
+        <v>100003</v>
+      </c>
+      <c r="D115" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E115" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="F115" s="0" t="n">
+        <v>100003</v>
+      </c>
+    </row>
+    <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A116" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B116" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C116" s="0" t="n">
+        <v>100004</v>
+      </c>
+      <c r="D116" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E116" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="F116" s="0" t="n">
+        <v>100004</v>
+      </c>
+    </row>
+    <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A117" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B117" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C117" s="0" t="n">
+        <v>100005</v>
+      </c>
+      <c r="D117" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E117" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="F117" s="0" t="n">
+        <v>100005</v>
+      </c>
+    </row>
+    <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A118" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B118" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C118" s="0" t="n">
+        <v>100006</v>
+      </c>
+      <c r="D118" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E118" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="F118" s="0" t="n">
+        <v>100006</v>
+      </c>
+    </row>
+    <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A119" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B119" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C119" s="0" t="n">
+        <v>100007</v>
+      </c>
+      <c r="D119" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E119" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="F119" s="0" t="n">
+        <v>100007</v>
+      </c>
+    </row>
+    <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A120" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B120" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C120" s="0" t="n">
+        <v>100008</v>
+      </c>
+      <c r="D120" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E120" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="F120" s="0" t="n">
+        <v>100008</v>
+      </c>
+    </row>
+    <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A121" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B121" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C121" s="0" t="n">
+        <v>100009</v>
+      </c>
+      <c r="D121" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E121" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="F121" s="0" t="n">
+        <v>100009</v>
+      </c>
+    </row>
+    <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A122" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B122" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C122" s="0" t="n">
+        <v>100010</v>
+      </c>
+      <c r="D122" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E122" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="F122" s="0" t="n">
+        <v>100010</v>
+      </c>
+    </row>
+    <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A123" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B123" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C123" s="0" t="n">
+        <v>100011</v>
+      </c>
+      <c r="D123" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E123" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="F123" s="0" t="n">
+        <v>100011</v>
+      </c>
+    </row>
+    <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A124" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B124" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C124" s="0" t="n">
+        <v>100012</v>
+      </c>
+      <c r="D124" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E124" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="F124" s="0" t="n">
+        <v>100012</v>
+      </c>
+    </row>
+    <row r="125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A125" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B125" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C125" s="0" t="n">
+        <v>950</v>
+      </c>
+      <c r="D125" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E125" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="F125" s="0" t="n">
+        <v>950</v>
+      </c>
+    </row>
+    <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A126" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B126" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C126" s="0" t="n">
+        <v>951</v>
+      </c>
+      <c r="D126" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E126" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="F126" s="0" t="n">
+        <v>951</v>
+      </c>
+    </row>
+    <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A127" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B127" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C127" s="0" t="n">
+        <v>952</v>
+      </c>
+      <c r="D127" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E127" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="F127" s="0" t="n">
+        <v>952</v>
+      </c>
+    </row>
+    <row r="128" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A128" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B128" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C128" s="0" t="n">
+        <v>953</v>
+      </c>
+      <c r="D128" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E128" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="F128" s="0" t="n">
+        <v>953</v>
+      </c>
+    </row>
+    <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A129" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B129" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C129" s="0" t="n">
+        <v>954</v>
+      </c>
+      <c r="D129" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E129" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="F129" s="0" t="n">
+        <v>954</v>
+      </c>
+    </row>
+    <row r="130" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A130" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B130" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C130" s="0" t="n">
+        <v>955</v>
+      </c>
+      <c r="D130" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E130" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="F130" s="0" t="n">
+        <v>955</v>
+      </c>
+    </row>
+    <row r="131" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A131" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B131" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C131" s="0" t="n">
+        <v>956</v>
+      </c>
+      <c r="D131" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E131" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="F131" s="0" t="n">
+        <v>956</v>
+      </c>
+    </row>
+    <row r="132" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A132" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B132" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C132" s="0" t="n">
+        <v>957</v>
+      </c>
+      <c r="D132" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E132" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="F132" s="0" t="n">
+        <v>957</v>
+      </c>
+    </row>
+    <row r="133" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A133" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B133" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C133" s="0" t="n">
+        <v>958</v>
+      </c>
+      <c r="D133" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E133" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="F133" s="0" t="n">
+        <v>958</v>
+      </c>
+    </row>
+    <row r="134" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A134" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B134" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C134" s="0" t="n">
+        <v>959</v>
+      </c>
+      <c r="D134" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E134" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="F134" s="0" t="n">
+        <v>959</v>
+      </c>
+    </row>
+    <row r="135" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A135" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B135" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C135" s="0" t="n">
+        <v>960</v>
+      </c>
+      <c r="D135" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E135" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="F135" s="0" t="n">
+        <v>960</v>
+      </c>
+    </row>
+    <row r="136" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A136" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B136" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C136" s="0" t="n">
+        <v>725</v>
+      </c>
+      <c r="D136" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E136" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="F136" s="0" t="n">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="137" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A137" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B137" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C137" s="0" t="n">
+        <v>726</v>
+      </c>
+      <c r="D137" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E137" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="F137" s="0" t="n">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="138" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A138" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B138" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C138" s="0" t="n">
+        <v>727</v>
+      </c>
+      <c r="D138" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E138" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="F138" s="0" t="n">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="139" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A139" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B139" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C139" s="0" t="n">
+        <v>728</v>
+      </c>
+      <c r="D139" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E139" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="F139" s="0" t="n">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="140" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A140" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B140" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C140" s="0" t="n">
+        <v>729</v>
+      </c>
+      <c r="D140" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E140" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="F140" s="0" t="n">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="141" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A141" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B141" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C141" s="0" t="n">
+        <v>730</v>
+      </c>
+      <c r="D141" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E141" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="F141" s="0" t="n">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="142" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A142" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B142" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C142" s="0" t="n">
+        <v>731</v>
+      </c>
+      <c r="D142" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E142" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="F142" s="0" t="n">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="143" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A143" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B143" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C143" s="0" t="n">
+        <v>732</v>
+      </c>
+      <c r="D143" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E143" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="F143" s="0" t="n">
+        <v>732</v>
+      </c>
+    </row>
+    <row r="144" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A144" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B144" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C144" s="0" t="n">
+        <v>733</v>
+      </c>
+      <c r="D144" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E144" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="F144" s="0" t="n">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="145" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A145" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B145" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C145" s="0" t="n">
+        <v>734</v>
+      </c>
+      <c r="D145" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E145" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="F145" s="0" t="n">
+        <v>734</v>
+      </c>
+    </row>
+    <row r="146" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A146" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B146" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C146" s="0" t="n">
+        <v>333</v>
+      </c>
+      <c r="D146" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E146" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="F146" s="0" t="n">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="147" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A147" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B147" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C147" s="0" t="n">
+        <v>334</v>
+      </c>
+      <c r="D147" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E147" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="F147" s="0" t="n">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="148" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A148" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B148" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C148" s="0" t="n">
+        <v>335</v>
+      </c>
+      <c r="D148" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E148" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="F148" s="0" t="n">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="149" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A149" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B149" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C149" s="0" t="n">
+        <v>336</v>
+      </c>
+      <c r="D149" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E149" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="F149" s="0" t="n">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="150" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A150" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B150" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C150" s="0" t="n">
+        <v>337</v>
+      </c>
+      <c r="D150" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E150" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="F150" s="0" t="n">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="151" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A151" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B151" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C151" s="0" t="n">
+        <v>338</v>
+      </c>
+      <c r="D151" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E151" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="F151" s="0" t="n">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="152" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A152" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B152" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C152" s="0" t="n">
+        <v>339</v>
+      </c>
+      <c r="D152" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E152" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="F152" s="0" t="n">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="153" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A153" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B153" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C153" s="0" t="n">
+        <v>340</v>
+      </c>
+      <c r="D153" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E153" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="F153" s="0" t="n">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="154" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A154" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B154" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C154" s="0" t="n">
+        <v>341</v>
+      </c>
+      <c r="D154" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E154" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="F154" s="0" t="n">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="155" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A155" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B155" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C155" s="0" t="n">
+        <v>342</v>
+      </c>
+      <c r="D155" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E155" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="F155" s="0" t="n">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="156" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A156" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B156" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C156" s="0" t="n">
+        <v>343</v>
+      </c>
+      <c r="D156" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E156" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="F156" s="0" t="n">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="157" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A157" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B157" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C157" s="0" t="n">
+        <v>344</v>
+      </c>
+      <c r="D157" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E157" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="F157" s="0" t="n">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="158" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A158" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B158" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C158" s="0" t="n">
+        <v>345</v>
+      </c>
+      <c r="D158" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E158" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="F158" s="0" t="n">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="159" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A159" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B159" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C159" s="0" t="n">
+        <v>346</v>
+      </c>
+      <c r="D159" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E159" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="F159" s="0" t="n">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="160" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A160" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B160" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C160" s="0" t="n">
+        <v>347</v>
+      </c>
+      <c r="D160" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E160" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="F160" s="0" t="n">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="161" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A161" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B161" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C161" s="0" t="n">
+        <v>348</v>
+      </c>
+      <c r="D161" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E161" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="F161" s="0" t="n">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="162" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A162" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B162" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C162" s="0" t="n">
+        <v>349</v>
+      </c>
+      <c r="D162" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E162" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="F162" s="0" t="n">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="163" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A163" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B163" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C163" s="0" t="n">
+        <v>350</v>
+      </c>
+      <c r="D163" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E163" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="F163" s="0" t="n">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="164" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A164" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B164" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C164" s="0" t="n">
+        <v>56789</v>
+      </c>
+      <c r="D164" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E164" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="F164" s="0" t="n">
+        <v>56789</v>
+      </c>
+    </row>
+    <row r="165" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A165" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B165" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C165" s="0" t="n">
+        <v>56790</v>
+      </c>
+      <c r="D165" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E165" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="F165" s="0" t="n">
+        <v>56790</v>
+      </c>
+    </row>
+    <row r="166" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A166" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B166" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C166" s="0" t="n">
+        <v>56791</v>
+      </c>
+      <c r="D166" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E166" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="F166" s="0" t="n">
+        <v>56791</v>
+      </c>
+    </row>
+    <row r="167" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A167" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B167" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C167" s="0" t="n">
+        <v>56792</v>
+      </c>
+      <c r="D167" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E167" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="F167" s="0" t="n">
+        <v>56792</v>
+      </c>
+    </row>
+    <row r="168" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A168" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B168" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C168" s="0" t="n">
+        <v>56793</v>
+      </c>
+      <c r="D168" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E168" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="F168" s="0" t="n">
+        <v>56793</v>
+      </c>
+    </row>
+    <row r="169" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A169" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B169" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C169" s="0" t="n">
+        <v>56794</v>
+      </c>
+      <c r="D169" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E169" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="F169" s="0" t="n">
+        <v>56794</v>
+      </c>
+    </row>
+    <row r="170" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A170" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B170" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C170" s="0" t="n">
+        <v>56795</v>
+      </c>
+      <c r="D170" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E170" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="F170" s="0" t="n">
+        <v>56795</v>
+      </c>
+    </row>
+    <row r="171" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A171" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B171" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C171" s="0" t="n">
+        <v>56796</v>
+      </c>
+      <c r="D171" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E171" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="F171" s="0" t="n">
+        <v>56796</v>
+      </c>
+    </row>
+    <row r="172" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A172" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B172" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C172" s="0" t="n">
+        <v>56797</v>
+      </c>
+      <c r="D172" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E172" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="F172" s="0" t="n">
+        <v>56797</v>
+      </c>
+    </row>
+    <row r="173" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A173" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B173" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C173" s="0" t="n">
+        <v>56798</v>
+      </c>
+      <c r="D173" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E173" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="F173" s="0" t="n">
+        <v>56798</v>
+      </c>
+    </row>
+    <row r="174" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A174" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B174" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C174" s="0" t="n">
+        <v>56799</v>
+      </c>
+      <c r="D174" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E174" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="F174" s="0" t="n">
+        <v>56799</v>
+      </c>
+    </row>
+    <row r="175" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A175" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B175" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C175" s="0" t="n">
+        <v>56800</v>
+      </c>
+      <c r="D175" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E175" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="F175" s="0" t="n">
+        <v>56800</v>
+      </c>
+    </row>
+    <row r="176" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A176" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B176" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C176" s="0" t="n">
+        <v>56801</v>
+      </c>
+      <c r="D176" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E176" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="F176" s="0" t="n">
+        <v>56801</v>
+      </c>
+    </row>
+    <row r="177" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A177" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B177" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C177" s="0" t="n">
+        <v>56802</v>
+      </c>
+      <c r="D177" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E177" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="F177" s="0" t="n">
+        <v>56802</v>
+      </c>
+    </row>
+    <row r="178" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A178" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B178" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C178" s="0" t="n">
+        <v>56803</v>
+      </c>
+      <c r="D178" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E178" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="F178" s="0" t="n">
+        <v>56803</v>
+      </c>
+    </row>
+    <row r="179" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A179" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B179" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C179" s="0" t="n">
+        <v>56804</v>
+      </c>
+      <c r="D179" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E179" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="F179" s="0" t="n">
+        <v>56804</v>
+      </c>
+    </row>
+    <row r="180" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A180" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B180" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C180" s="0" t="n">
+        <v>56805</v>
+      </c>
+      <c r="D180" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E180" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="F180" s="0" t="n">
+        <v>56805</v>
+      </c>
+    </row>
+    <row r="181" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A181" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B181" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C181" s="0" t="n">
+        <v>56806</v>
+      </c>
+      <c r="D181" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E181" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="F181" s="0" t="n">
+        <v>56806</v>
+      </c>
+    </row>
+    <row r="182" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A182" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B182" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C182" s="0" t="n">
+        <v>56807</v>
+      </c>
+      <c r="D182" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E182" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="F182" s="0" t="n">
+        <v>56807</v>
+      </c>
+    </row>
+    <row r="183" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A183" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B183" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C183" s="0" t="n">
+        <v>56808</v>
+      </c>
+      <c r="D183" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E183" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="F183" s="0" t="n">
+        <v>56808</v>
+      </c>
+    </row>
+    <row r="184" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A184" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B184" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C184" s="0" t="n">
+        <v>56809</v>
+      </c>
+      <c r="D184" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E184" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="F184" s="0" t="n">
+        <v>56809</v>
+      </c>
+    </row>
+    <row r="185" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A185" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B185" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C185" s="0" t="n">
         <v>56810</v>
       </c>
-      <c r="D105" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="E105" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="F105" s="0" t="n">
+      <c r="D185" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E185" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="F185" s="0" t="n">
         <v>56810</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Changes to cater to forms, dates and Math questions
</commit_message>
<xml_diff>
--- a/src/main/resources/questions/Numbers.xlsx
+++ b/src/main/resources/questions/Numbers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Nikhil KM\AmoghLMS\LearningManagementSystem\src\main\resources\questions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{5F53531C-D110-4A3B-83DF-D9339345849C}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{03784129-27A8-435B-BB12-34F61EA5AC33}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="993" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -429,14 +429,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F185"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A165" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D185" sqref="D185"/>
+    <sheetView tabSelected="1" topLeftCell="A172" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J183" sqref="J183"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13.33203125"/>
-    <col min="2" max="2" width="20.109375"/>
+    <col min="2" max="2" width="24.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.77734375"/>
     <col min="4" max="4" width="13.109375"/>
     <col min="5" max="5" width="18.5546875"/>

</xml_diff>